<commit_message>
modificacion de tabla se agregan description de atributos
</commit_message>
<xml_diff>
--- a/tabla platzistore.xlsx
+++ b/tabla platzistore.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>CARRITO</t>
   </si>
@@ -63,6 +63,33 @@
   </si>
   <si>
     <t>1-1</t>
+  </si>
+  <si>
+    <t>Atributo</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Obligatorio</t>
+  </si>
+  <si>
+    <t>llave prim</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Serial</t>
+  </si>
+  <si>
+    <t>cuentaPlatzi</t>
+  </si>
+  <si>
+    <t>varchar(60)</t>
   </si>
 </sst>
 </file>
@@ -113,11 +140,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +608,57 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:D9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>